<commit_message>
all 3 persona til cpc test user
</commit_message>
<xml_diff>
--- a/DataSheet/FOS7_AfterPostSanction.xlsx
+++ b/DataSheet/FOS7_AfterPostSanction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B135982-D65D-4639-A990-4D1CA9569EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC55FF68-A082-4B25-B378-54EBB84C36F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
     <t>//android.view.View[contains(@content-desc,"Post Sanction")]</t>
   </si>
   <si>
-    <t>MF24121100006530</t>
+    <t>MF24121500006171</t>
   </si>
 </sst>
 </file>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,8 +4587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4711,16 +4711,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>80</v>

</xml_diff>